<commit_message>
adiciona tratamento de exceções ao enviar arquivos e ajusta a paralelização do processamento
</commit_message>
<xml_diff>
--- a/pontuacoes_servicos.xlsx
+++ b/pontuacoes_servicos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,65 +503,199 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Acessar_agência_virtual.txt</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Acessar_dados_do_portal_da_transparência.txt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Acessar_editais_de_concurso_público_e_processos_seletivos.txt</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>1.5</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>1.5</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>